<commit_message>
Cleaned the repository, keeping only necessary files, and restructuring the results and plots folders
</commit_message>
<xml_diff>
--- a/results/Sobol_composite CCB.xlsx
+++ b/results/Sobol_composite CCB.xlsx
@@ -477,10 +477,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.03153561597069461</v>
+        <v>0.03152867426506853</v>
       </c>
       <c r="E2" t="n">
-        <v>0.03246849461509092</v>
+        <v>0.03247278806658015</v>
       </c>
     </row>
     <row r="3">
@@ -523,10 +523,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.9667966455832187</v>
+        <v>0.9669225664469602</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9676929414250738</v>
+        <v>0.9678280840786686</v>
       </c>
     </row>
     <row r="5">
@@ -546,10 +546,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1.058784503841472e-07</v>
+        <v>5.478448198438688e-08</v>
       </c>
       <c r="E5" t="n">
-        <v>3.843680085559115e-08</v>
+        <v>3.843649510071133e-08</v>
       </c>
     </row>
     <row r="6">
@@ -592,10 +592,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>9.669093401623241e-07</v>
+        <v>1.790121146373665e-06</v>
       </c>
       <c r="E7" t="n">
-        <v>1.846465643824241e-06</v>
+        <v>1.846153151161725e-06</v>
       </c>
     </row>
     <row r="8">
@@ -615,10 +615,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.0001152663841241229</v>
+        <v>0.0001110025731964453</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0001425894872388249</v>
+        <v>0.0001425875061118723</v>
       </c>
     </row>
     <row r="9">
@@ -638,10 +638,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.0003256771713309216</v>
+        <v>0.0003222373793821501</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0003620058416811836</v>
+        <v>0.0003621757543964986</v>
       </c>
     </row>
     <row r="10">
@@ -684,10 +684,10 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.0001209463883616704</v>
+        <v>0.0001231196748913675</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0001514953991804979</v>
+        <v>0.0001517665460525593</v>
       </c>
     </row>
     <row r="12">
@@ -707,10 +707,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.001507953311683096</v>
+        <v>0.001475488146219165</v>
       </c>
       <c r="E12" t="n">
-        <v>0.001577628410917391</v>
+        <v>0.00157753395837439</v>
       </c>
     </row>
     <row r="13">
@@ -753,10 +753,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.09328774697488056</v>
+        <v>0.09331672935525699</v>
       </c>
       <c r="E14" t="n">
-        <v>0.09338335467414463</v>
+        <v>0.09338239515312979</v>
       </c>
     </row>
     <row r="15">
@@ -776,10 +776,10 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>-2.471164718347308e-07</v>
+        <v>4.304592254037789e-08</v>
       </c>
       <c r="E15" t="n">
-        <v>7.611423535041819e-08</v>
+        <v>7.610203471194547e-08</v>
       </c>
     </row>
     <row r="16">
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>-5.946692039186194e-09</v>
+        <v>3.143056735785347e-09</v>
       </c>
       <c r="E17" t="n">
-        <v>4.596902578443971e-10</v>
+        <v>4.595435607885807e-10</v>
       </c>
     </row>
     <row r="18">
@@ -845,10 +845,10 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.1912347941504496</v>
+        <v>0.1915822842741306</v>
       </c>
       <c r="E18" t="n">
-        <v>0.232741454547814</v>
+        <v>0.2326976219508576</v>
       </c>
     </row>
     <row r="19">
@@ -868,10 +868,10 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.5211336139098187</v>
+        <v>0.5208044101611119</v>
       </c>
       <c r="E19" t="n">
-        <v>0.5755514465875111</v>
+        <v>0.5756503975091606</v>
       </c>
     </row>
     <row r="20">
@@ -914,10 +914,10 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.1299361727519368</v>
+        <v>0.1295186339205768</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1605381077546346</v>
+        <v>0.1608013301712574</v>
       </c>
     </row>
     <row r="22">
@@ -937,10 +937,10 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.03153442010405258</v>
+        <v>0.03152131263016886</v>
       </c>
       <c r="E22" t="n">
-        <v>0.03245977579255492</v>
+        <v>0.03246383359135453</v>
       </c>
     </row>
     <row r="23">
@@ -983,10 +983,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.9632323082408174</v>
+        <v>0.9633546058399578</v>
       </c>
       <c r="E24" t="n">
-        <v>0.9641265098868251</v>
+        <v>0.9642540359987541</v>
       </c>
     </row>
     <row r="25">
@@ -1006,10 +1006,10 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>7.859845703160869e-08</v>
+        <v>2.988686901270778e-08</v>
       </c>
       <c r="E25" t="n">
-        <v>1.739781242106183e-08</v>
+        <v>1.739753869590781e-08</v>
       </c>
     </row>
     <row r="26">
@@ -1052,10 +1052,10 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>5.142375921268753e-07</v>
+        <v>1.197251797443755e-06</v>
       </c>
       <c r="E27" t="n">
-        <v>1.236256368805198e-06</v>
+        <v>1.236038022026848e-06</v>
       </c>
     </row>
     <row r="28">
@@ -1075,10 +1075,10 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.0008516072015306379</v>
+        <v>0.0008424264892473845</v>
       </c>
       <c r="E28" t="n">
-        <v>0.001040964344474445</v>
+        <v>0.001040923521786564</v>
       </c>
     </row>
     <row r="29">
@@ -1098,10 +1098,10 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.002359102560988276</v>
+        <v>0.002349382973208291</v>
       </c>
       <c r="E29" t="n">
-        <v>0.00260790041482767</v>
+        <v>0.002608842710053543</v>
       </c>
     </row>
     <row r="30">
@@ -1144,10 +1144,10 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.0006728789187348313</v>
+        <v>0.0006767160068664465</v>
       </c>
       <c r="E31" t="n">
-        <v>0.0008361402600897291</v>
+        <v>0.0008376306024780586</v>
       </c>
     </row>
     <row r="32">
@@ -1167,10 +1167,10 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.03234513801026135</v>
+        <v>0.03233606662732572</v>
       </c>
       <c r="E32" t="n">
-        <v>0.0332750274869494</v>
+        <v>0.03327940067603422</v>
       </c>
     </row>
     <row r="33">
@@ -1213,10 +1213,10 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.9651672060936886</v>
+        <v>0.9652916221474339</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9660622857513241</v>
+        <v>0.9661952532501226</v>
       </c>
     </row>
     <row r="35">
@@ -1236,10 +1236,10 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>9.397236776224196e-08</v>
+        <v>6.154004135409141e-08</v>
       </c>
       <c r="E35" t="n">
-        <v>4.316977505289601e-08</v>
+        <v>4.316934030038275e-08</v>
       </c>
     </row>
     <row r="36">
@@ -1282,10 +1282,10 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>2.615156067460584e-07</v>
+        <v>8.250850099589941e-07</v>
       </c>
       <c r="E37" t="n">
-        <v>8.609650202522001e-07</v>
+        <v>8.608175769851677e-07</v>
       </c>
     </row>
     <row r="38">
@@ -1305,10 +1305,10 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.0002932428201739054</v>
+        <v>0.0002873599731884779</v>
       </c>
       <c r="E38" t="n">
-        <v>0.0003573756586887759</v>
+        <v>0.0003573631988097969</v>
       </c>
     </row>
     <row r="39">
@@ -1328,10 +1328,10 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.0008139217120394152</v>
+        <v>0.00080849541570621</v>
       </c>
       <c r="E39" t="n">
-        <v>0.0008959989110323383</v>
+        <v>0.0008963208783202668</v>
       </c>
     </row>
     <row r="40">
@@ -1374,10 +1374,10 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.0002253023549856609</v>
+        <v>0.0002280596558474274</v>
       </c>
       <c r="E41" t="n">
-        <v>0.0002811545997290932</v>
+        <v>0.0002816572432886632</v>
       </c>
     </row>
     <row r="42">
@@ -1397,10 +1397,10 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.03103545343076839</v>
+        <v>0.03102795755520045</v>
       </c>
       <c r="E42" t="n">
-        <v>0.03196801202863241</v>
+        <v>0.03197218449716255</v>
       </c>
     </row>
     <row r="43">
@@ -1443,10 +1443,10 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.9669103720273562</v>
+        <v>0.9670359258268386</v>
       </c>
       <c r="E44" t="n">
-        <v>0.9678068033216838</v>
+        <v>0.967941011302884</v>
       </c>
     </row>
     <row r="45">
@@ -1466,10 +1466,10 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>7.008739431238591e-08</v>
+        <v>1.78718084644895e-08</v>
       </c>
       <c r="E45" t="n">
-        <v>9.486782965417684e-09</v>
+        <v>9.486665275060907e-09</v>
       </c>
     </row>
     <row r="46">
@@ -1512,10 +1512,10 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>6.897852777726034e-07</v>
+        <v>1.429132951526767e-06</v>
       </c>
       <c r="E47" t="n">
-        <v>1.477246668128465e-06</v>
+        <v>1.476995210954716e-06</v>
       </c>
     </row>
     <row r="48">
@@ -1535,10 +1535,10 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.0001637354480504567</v>
+        <v>0.0001588184769055738</v>
       </c>
       <c r="E48" t="n">
-        <v>0.0002027904379636927</v>
+        <v>0.0002027873494665007</v>
       </c>
     </row>
     <row r="49">
@@ -1558,10 +1558,10 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.0005938049402491403</v>
+        <v>0.0005891671239398874</v>
       </c>
       <c r="E49" t="n">
-        <v>0.0006458397157028422</v>
+        <v>0.0006460923857445842</v>
       </c>
     </row>
     <row r="50">
@@ -1604,10 +1604,10 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.0001716188087904062</v>
+        <v>0.0001741047960137347</v>
       </c>
       <c r="E51" t="n">
-        <v>0.0002145044781385741</v>
+        <v>0.0002148881877967148</v>
       </c>
     </row>
     <row r="52">
@@ -1627,10 +1627,10 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.03311684121970455</v>
+        <v>0.03311349093060512</v>
       </c>
       <c r="E52" t="n">
-        <v>0.03405116788455223</v>
+        <v>0.03405591510436534</v>
       </c>
     </row>
     <row r="53">
@@ -1673,10 +1673,10 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.9658252533821632</v>
+        <v>0.9659517992178833</v>
       </c>
       <c r="E54" t="n">
-        <v>0.9667196253303774</v>
+        <v>0.9668594289187364</v>
       </c>
     </row>
     <row r="55">
@@ -1696,10 +1696,10 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>5.020504572021985e-09</v>
+        <v>3.10812722204093e-09</v>
       </c>
       <c r="E55" t="n">
-        <v>7.197501156319162e-10</v>
+        <v>7.197476913986338e-10</v>
       </c>
     </row>
     <row r="56">
@@ -1742,10 +1742,10 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>-5.128017007737958e-08</v>
+        <v>4.875011103233837e-09</v>
       </c>
       <c r="E57" t="n">
-        <v>8.829863473308657e-09</v>
+        <v>8.82841292268661e-09</v>
       </c>
     </row>
     <row r="58">
@@ -1765,10 +1765,10 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>9.690110348274944e-08</v>
+        <v>-2.605279123551435e-08</v>
       </c>
       <c r="E58" t="n">
-        <v>9.538048710744832e-08</v>
+        <v>9.538010634525989e-08</v>
       </c>
     </row>
     <row r="59">
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>3.212308825039537e-07</v>
+        <v>2.370236012648282e-07</v>
       </c>
       <c r="E59" t="n">
-        <v>2.411786592305175e-07</v>
+        <v>2.412993050328337e-07</v>
       </c>
     </row>
     <row r="60">
@@ -1834,10 +1834,10 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>4.253187161202927e-08</v>
+        <v>1.104819520404359e-07</v>
       </c>
       <c r="E61" t="n">
-        <v>1.074687292111577e-07</v>
+        <v>1.076616111708045e-07</v>
       </c>
     </row>
     <row r="62">
@@ -1857,10 +1857,10 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.004970291074895866</v>
+        <v>0.004964292742250733</v>
       </c>
       <c r="E62" t="n">
-        <v>0.005926542283213622</v>
+        <v>0.005926194277710036</v>
       </c>
     </row>
     <row r="63">
@@ -1903,10 +1903,10 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0.9903385069002735</v>
+        <v>0.990470442653995</v>
       </c>
       <c r="E64" t="n">
-        <v>0.9912593097749092</v>
+        <v>0.9913791772882952</v>
       </c>
     </row>
     <row r="65">
@@ -1926,10 +1926,10 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>6.717078973528343e-05</v>
+        <v>6.62047829831332e-05</v>
       </c>
       <c r="E65" t="n">
-        <v>6.683805491132715e-05</v>
+        <v>6.683610851992789e-05</v>
       </c>
     </row>
     <row r="66">
@@ -1972,10 +1972,10 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>8.622593774947257e-09</v>
+        <v>4.788129282627179e-07</v>
       </c>
       <c r="E67" t="n">
-        <v>5.026777764762369e-07</v>
+        <v>5.025832919078942e-07</v>
       </c>
     </row>
     <row r="68">
@@ -1995,10 +1995,10 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>8.9947517867043e-05</v>
+        <v>7.842938862393597e-05</v>
       </c>
       <c r="E68" t="n">
-        <v>0.0002874169579656936</v>
+        <v>0.0002879899196287711</v>
       </c>
     </row>
     <row r="69">
@@ -2018,10 +2018,10 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0.0002374349229070527</v>
+        <v>0.0002315701660516728</v>
       </c>
       <c r="E69" t="n">
-        <v>0.0007028473035783007</v>
+        <v>0.0007030587265269982</v>
       </c>
     </row>
     <row r="70">
@@ -2064,10 +2064,10 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0.002575958640133949</v>
+        <v>0.002580629021938413</v>
       </c>
       <c r="E71" t="n">
-        <v>0.003193794352847657</v>
+        <v>0.003199450696079281</v>
       </c>
     </row>
     <row r="72">
@@ -2087,10 +2087,10 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.03221319657117862</v>
+        <v>0.03220282669064249</v>
       </c>
       <c r="E72" t="n">
-        <v>0.03314158623439658</v>
+        <v>0.03314588441963309</v>
       </c>
     </row>
     <row r="73">
@@ -2133,10 +2133,10 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0.9645343159099546</v>
+        <v>0.9646587482764758</v>
       </c>
       <c r="E74" t="n">
-        <v>0.965429250969484</v>
+        <v>0.9655606054349972</v>
       </c>
     </row>
     <row r="75">
@@ -2156,10 +2156,10 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>5.822618265514602e-07</v>
+        <v>5.101934185805416e-07</v>
       </c>
       <c r="E75" t="n">
-        <v>4.581654020826932e-07</v>
+        <v>4.581598907765387e-07</v>
       </c>
     </row>
     <row r="76">
@@ -2202,10 +2202,10 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>3.335705334245563e-06</v>
+        <v>4.664182564780058e-06</v>
       </c>
       <c r="E77" t="n">
-        <v>4.752441583670661e-06</v>
+        <v>4.751620202327093e-06</v>
       </c>
     </row>
     <row r="78">
@@ -2225,10 +2225,10 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0.0004492064102287967</v>
+        <v>0.0004421731634407361</v>
       </c>
       <c r="E78" t="n">
-        <v>0.0005475915646016231</v>
+        <v>0.0005475712595412996</v>
       </c>
     </row>
     <row r="79">
@@ -2248,10 +2248,10 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.001250636140309144</v>
+        <v>0.001243825224572</v>
       </c>
       <c r="E79" t="n">
-        <v>0.001377471977705306</v>
+        <v>0.001377957188340125</v>
       </c>
     </row>
     <row r="80">
@@ -2294,10 +2294,10 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0.0003412614363776532</v>
+        <v>0.0003444385036674718</v>
       </c>
       <c r="E81" t="n">
-        <v>0.0004250580939052002</v>
+        <v>0.0004258173328285274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>